<commit_message>
negligible partitioning zeroed and spin-up
to reduce stiffness when gas-particle partitioning components reduce to very small concentrations, gas-particle partitioning of these species is now turned off in partit_var.py. Furthermore, users may now specify to spin-up a simulation.
</commit_message>
<xml_diff>
--- a/PyCHAM/input/ambient_constrained_ex/ambient_constrained_ex_obs.xlsx
+++ b/PyCHAM/input/ambient_constrained_ex/ambient_constrained_ex_obs.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Psymo\Desktop\PyCHAM\PyCHAM\PyCHAM\input\ambient_constrained_ex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/PyCHAM/PyCHAM/input/ambient_constrained_ex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D0BBFA-B774-4FD4-9D8C-C977972123F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CE9166-A355-2548-A46B-A773746E0848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6972" yWindow="768" windowWidth="12900" windowHeight="10392" xr2:uid="{7C74D523-2B60-6A4A-ACEB-A35EBE6838C7}"/>
+    <workbookView xWindow="6980" yWindow="760" windowWidth="12900" windowHeight="10400" xr2:uid="{7C74D523-2B60-6A4A-ACEB-A35EBE6838C7}"/>
   </bookViews>
   <sheets>
     <sheet name="PyCHAMobs" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Time (s)</t>
   </si>
@@ -40,9 +52,6 @@
   </si>
   <si>
     <t>APINENE</t>
-  </si>
-  <si>
-    <t>BENZENE</t>
   </si>
 </sst>
 </file>
@@ -395,15 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C87549-F558-ED41-B912-C5D536F6DDBE}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F73"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,11 +428,8 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -433,17 +439,14 @@
       <c r="C2">
         <v>678441994290.95752</v>
       </c>
-      <c r="D2">
-        <v>3354657831.5493841</v>
+      <c r="D2" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E2" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F2" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>300</v>
       </c>
@@ -453,17 +456,14 @@
       <c r="C3">
         <v>692461459855.64148</v>
       </c>
-      <c r="D3">
-        <v>4030596349.8466477</v>
+      <c r="D3" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E3" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F3" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>600</v>
       </c>
@@ -473,17 +473,14 @@
       <c r="C4">
         <v>710236139410.86584</v>
       </c>
-      <c r="D4">
-        <v>-500695198.73871398</v>
+      <c r="D4" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E4" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F4" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>900</v>
       </c>
@@ -493,17 +490,14 @@
       <c r="C5">
         <v>680695122685.28174</v>
       </c>
-      <c r="D5">
-        <v>-1702363675.7116277</v>
+      <c r="D5" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E5" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F5" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1200</v>
       </c>
@@ -513,17 +507,14 @@
       <c r="C6">
         <v>654909319950.23792</v>
       </c>
-      <c r="D6">
-        <v>1677328915.7746921</v>
+      <c r="D6" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E6" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F6" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1500</v>
       </c>
@@ -533,17 +524,14 @@
       <c r="C7">
         <v>674436432701.04773</v>
       </c>
-      <c r="D7">
-        <v>2979136432.495348</v>
+      <c r="D7" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E7" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F7" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1800</v>
       </c>
@@ -553,17 +541,14 @@
       <c r="C8">
         <v>706480925420.32544</v>
       </c>
-      <c r="D8">
-        <v>-125173799.68467849</v>
+      <c r="D8" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E8" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F8" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2100</v>
       </c>
@@ -573,17 +558,14 @@
       <c r="C9">
         <v>728010818966.09009</v>
       </c>
-      <c r="D9">
-        <v>-2653684553.3151841</v>
+      <c r="D9" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E9" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F9" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2400</v>
       </c>
@@ -593,17 +575,14 @@
       <c r="C10">
         <v>735521246947.17078</v>
       </c>
-      <c r="D10">
-        <v>-3179414511.9908338</v>
+      <c r="D10" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E10" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F10" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2700</v>
       </c>
@@ -613,17 +592,14 @@
       <c r="C11">
         <v>732266728155.36926</v>
       </c>
-      <c r="D11">
-        <v>-4606395828.3961687</v>
+      <c r="D11" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E11" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F11" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3000</v>
       </c>
@@ -633,17 +609,14 @@
       <c r="C12">
         <v>715493438997.62219</v>
       </c>
-      <c r="D12">
-        <v>-6659246143.2248964</v>
+      <c r="D12" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E12" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F12" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3300</v>
       </c>
@@ -653,17 +626,14 @@
       <c r="C13">
         <v>672433651906.0929</v>
       </c>
-      <c r="D13">
-        <v>-8261470779.1887808</v>
+      <c r="D13" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E13" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F13" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3600</v>
       </c>
@@ -673,17 +643,14 @@
       <c r="C14">
         <v>651654801158.43628</v>
       </c>
-      <c r="D14">
-        <v>-7260080381.7113523</v>
+      <c r="D14" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E14" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F14" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3900</v>
       </c>
@@ -693,17 +660,14 @@
       <c r="C15">
         <v>662169400331.94922</v>
       </c>
-      <c r="D15">
-        <v>-8611957418.3058796</v>
+      <c r="D15" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E15" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F15" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4200</v>
       </c>
@@ -713,17 +677,14 @@
       <c r="C16">
         <v>662419747931.3186</v>
       </c>
-      <c r="D16">
-        <v>-9713486855.5310516</v>
+      <c r="D16" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E16" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F16" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4500</v>
       </c>
@@ -733,17 +694,14 @@
       <c r="C17">
         <v>673685389902.9397</v>
       </c>
-      <c r="D17">
-        <v>-8611957418.3058796</v>
+      <c r="D17" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E17" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F17" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4800</v>
       </c>
@@ -753,17 +711,14 @@
       <c r="C18">
         <v>678942689489.69617</v>
       </c>
-      <c r="D18">
-        <v>-9763556375.4049225</v>
+      <c r="D18" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E18" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F18" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5100</v>
       </c>
@@ -773,17 +728,14 @@
       <c r="C19">
         <v>659665924338.25574</v>
       </c>
-      <c r="D19">
-        <v>-9838660655.2157307</v>
+      <c r="D19" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E19" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F19" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5400</v>
       </c>
@@ -793,17 +745,14 @@
       <c r="C20">
         <v>678191646691.58813</v>
       </c>
-      <c r="D20">
-        <v>-7986088419.8824883</v>
+      <c r="D20" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E20" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F20" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>5700</v>
       </c>
@@ -813,17 +762,14 @@
       <c r="C21">
         <v>689206941063.83984</v>
       </c>
-      <c r="D21">
-        <v>-4531291548.5853615</v>
+      <c r="D21" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E21" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F21" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6000</v>
       </c>
@@ -833,17 +779,14 @@
       <c r="C22">
         <v>657663143543.30078</v>
       </c>
-      <c r="D22">
-        <v>-1151598957.0990422</v>
+      <c r="D22" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E22" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F22" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6300</v>
       </c>
@@ -853,17 +796,14 @@
       <c r="C23">
         <v>654658972350.86853</v>
       </c>
-      <c r="D23">
-        <v>6559107103.4771538</v>
+      <c r="D23" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E23" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F23" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6600</v>
       </c>
@@ -873,17 +813,14 @@
       <c r="C24">
         <v>675187475499.15576</v>
       </c>
-      <c r="D24">
-        <v>11791371930.296713</v>
+      <c r="D24" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E24" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F24" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6900</v>
       </c>
@@ -893,17 +830,14 @@
       <c r="C25">
         <v>680194427486.54297</v>
       </c>
-      <c r="D25">
-        <v>12542414728.404785</v>
+      <c r="D25" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E25" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F25" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7200</v>
       </c>
@@ -913,17 +847,14 @@
       <c r="C26">
         <v>682697903480.23657</v>
       </c>
-      <c r="D26">
-        <v>12617519008.215593</v>
+      <c r="D26" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E26" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F26" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7500</v>
       </c>
@@ -933,17 +864,14 @@
       <c r="C27">
         <v>702725711429.78503</v>
       </c>
-      <c r="D27">
-        <v>9388034976.3508873</v>
+      <c r="D27" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E27" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F27" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>7800</v>
       </c>
@@ -953,17 +881,14 @@
       <c r="C28">
         <v>695465631048.07373</v>
       </c>
-      <c r="D28">
-        <v>5883168585.1798887</v>
+      <c r="D28" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E28" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F28" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8100</v>
       </c>
@@ -973,17 +898,14 @@
       <c r="C29">
         <v>679193037089.06555</v>
       </c>
-      <c r="D29">
-        <v>-3504866391.1709981</v>
+      <c r="D29" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E29" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F29" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>8400</v>
       </c>
@@ -993,17 +915,14 @@
       <c r="C30">
         <v>692711807455.01086</v>
       </c>
-      <c r="D30">
-        <v>-10514599173.512993</v>
+      <c r="D30" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E30" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F30" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>8700</v>
       </c>
@@ -1013,17 +932,14 @@
       <c r="C31">
         <v>702225016231.04639</v>
       </c>
-      <c r="D31">
-        <v>-12492345208.530914</v>
+      <c r="D31" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E31" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F31" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>9000</v>
       </c>
@@ -1033,17 +949,14 @@
       <c r="C32">
         <v>698720149839.87537</v>
       </c>
-      <c r="D32">
-        <v>-9588313055.8463726</v>
+      <c r="D32" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E32" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F32" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>9300</v>
       </c>
@@ -1053,17 +966,14 @@
       <c r="C33">
         <v>702725711429.78503</v>
       </c>
-      <c r="D33">
-        <v>-4356048229.0268116</v>
+      <c r="D33" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E33" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F33" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>9600</v>
       </c>
@@ -1073,17 +983,14 @@
       <c r="C34">
         <v>714241701000.77551</v>
       </c>
-      <c r="D34">
-        <v>-1151598957.0990422</v>
+      <c r="D34" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E34" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F34" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>9900</v>
       </c>
@@ -1093,17 +1000,14 @@
       <c r="C35">
         <v>706230577820.95605</v>
       </c>
-      <c r="D35">
-        <v>3229484031.8647051</v>
+      <c r="D35" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E35" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F35" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>10200</v>
       </c>
@@ -1113,17 +1017,14 @@
       <c r="C36">
         <v>704478144625.37061</v>
       </c>
-      <c r="D36">
-        <v>7335184661.5221596</v>
+      <c r="D36" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E36" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F36" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>10500</v>
       </c>
@@ -1133,17 +1034,14 @@
       <c r="C37">
         <v>714241701000.77551</v>
       </c>
-      <c r="D37">
-        <v>9613347815.783308</v>
+      <c r="D37" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E37" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F37" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>10800</v>
       </c>
@@ -1153,17 +1051,14 @@
       <c r="C38">
         <v>698970497439.24475</v>
       </c>
-      <c r="D38">
-        <v>6333794264.0447321</v>
+      <c r="D38" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E38" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F38" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>11100</v>
       </c>
@@ -1173,17 +1068,14 @@
       <c r="C39">
         <v>688205550666.3623</v>
       </c>
-      <c r="D39">
-        <v>1376911796.5314634</v>
+      <c r="D39" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E39" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F39" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>11400</v>
       </c>
@@ -1193,17 +1085,14 @@
       <c r="C40">
         <v>701473973432.93823</v>
       </c>
-      <c r="D40">
-        <v>275382359.30629265</v>
+      <c r="D40" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E40" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F40" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>11700</v>
       </c>
@@ -1213,17 +1102,14 @@
       <c r="C41">
         <v>696216673846.18176</v>
       </c>
-      <c r="D41">
-        <v>-400556158.99097121</v>
+      <c r="D41" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E41" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F41" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>12000</v>
       </c>
@@ -1233,17 +1119,14 @@
       <c r="C42">
         <v>706731273019.69482</v>
       </c>
-      <c r="D42">
-        <v>-3529901151.1079335</v>
+      <c r="D42" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E42" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F42" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>12300</v>
       </c>
@@ -1253,17 +1136,14 @@
       <c r="C43">
         <v>732767423354.10791</v>
       </c>
-      <c r="D43">
-        <v>-6709315663.0987682</v>
+      <c r="D43" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E43" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F43" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>12600</v>
       </c>
@@ -1273,17 +1153,14 @@
       <c r="C44">
         <v>731014990158.52246</v>
       </c>
-      <c r="D44">
-        <v>-4831708667.8285904</v>
+      <c r="D44" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E44" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F44" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>12900</v>
       </c>
@@ -1293,17 +1170,14 @@
       <c r="C45">
         <v>693963545451.85754</v>
       </c>
-      <c r="D45">
-        <v>-2027815554.8917918</v>
+      <c r="D45" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E45" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F45" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>13200</v>
       </c>
@@ -1313,17 +1187,14 @@
       <c r="C46">
         <v>664923223925.01208</v>
       </c>
-      <c r="D46">
-        <v>-1502085596.2161419</v>
+      <c r="D46" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E46" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F46" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>13500</v>
       </c>
@@ -1333,17 +1204,14 @@
       <c r="C47">
         <v>682447555880.86719</v>
       </c>
-      <c r="D47">
-        <v>-4356048229.0268116</v>
+      <c r="D47" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E47" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F47" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>13800</v>
       </c>
@@ -1353,17 +1221,14 @@
       <c r="C48">
         <v>702725711429.78503</v>
       </c>
-      <c r="D48">
-        <v>-3880387790.2250333</v>
+      <c r="D48" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E48" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F48" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>14100</v>
       </c>
@@ -1373,17 +1238,14 @@
       <c r="C49">
         <v>695715978647.44312</v>
       </c>
-      <c r="D49">
-        <v>525729958.6756497</v>
+      <c r="D49" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E49" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F49" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>14400</v>
       </c>
@@ -1393,17 +1255,14 @@
       <c r="C50">
         <v>667426699918.70581</v>
       </c>
-      <c r="D50">
-        <v>1376911796.5314634</v>
+      <c r="D50" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E50" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F50" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>14700</v>
       </c>
@@ -1413,17 +1272,14 @@
       <c r="C51">
         <v>663170790729.42664</v>
       </c>
-      <c r="D51">
-        <v>2403336953.945827</v>
+      <c r="D51" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E51" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F51" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>15000</v>
       </c>
@@ -1433,17 +1289,14 @@
       <c r="C52">
         <v>678942689489.69617</v>
       </c>
-      <c r="D52">
-        <v>2253128394.324213</v>
+      <c r="D52" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E52" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F52" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>15300</v>
       </c>
@@ -1453,17 +1306,14 @@
       <c r="C53">
         <v>702976059029.15442</v>
       </c>
-      <c r="D53">
-        <v>5432542906.3150463</v>
+      <c r="D53" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E53" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F53" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>15600</v>
       </c>
@@ -1473,17 +1323,14 @@
       <c r="C54">
         <v>725256995373.02722</v>
       </c>
-      <c r="D54">
-        <v>8261470779.1887808</v>
+      <c r="D54" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E54" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F54" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>15900</v>
       </c>
@@ -1493,17 +1340,14 @@
       <c r="C55">
         <v>713991353401.40613</v>
       </c>
-      <c r="D55">
-        <v>6734350423.0357037</v>
+      <c r="D55" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E55" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F55" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>16200</v>
       </c>
@@ -1513,17 +1357,14 @@
       <c r="C56">
         <v>696717369044.92053</v>
       </c>
-      <c r="D56">
-        <v>2578580273.5043769</v>
+      <c r="D56" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E56" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F56" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>16500</v>
       </c>
@@ -1533,17 +1374,14 @@
       <c r="C57">
         <v>678191646691.58813</v>
       </c>
-      <c r="D57">
-        <v>-751042798.10807097</v>
+      <c r="D57" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E57" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F57" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>16800</v>
       </c>
@@ -1553,17 +1391,14 @@
       <c r="C58">
         <v>667426699918.70581</v>
       </c>
-      <c r="D58">
-        <v>150208559.62161419</v>
+      <c r="D58" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E58" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F58" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>17100</v>
       </c>
@@ -1573,17 +1408,14 @@
       <c r="C59">
         <v>653407234354.02185</v>
       </c>
-      <c r="D59">
-        <v>2428371713.8827629</v>
+      <c r="D59" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E59" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F59" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>17400</v>
       </c>
@@ -1593,17 +1425,14 @@
       <c r="C60">
         <v>638636725991.22974</v>
       </c>
-      <c r="D60">
-        <v>1101529437.2251706</v>
+      <c r="D60" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E60" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F60" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>17700</v>
       </c>
@@ -1613,17 +1442,14 @@
       <c r="C61">
         <v>673935737502.30908</v>
       </c>
-      <c r="D61">
-        <v>1401946556.4683993</v>
+      <c r="D61" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E61" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F61" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>18000</v>
       </c>
@@ -1633,17 +1459,14 @@
       <c r="C62">
         <v>692461459855.64148</v>
       </c>
-      <c r="D62">
-        <v>3705144470.6664834</v>
+      <c r="D62" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E62" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F62" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>18300</v>
       </c>
@@ -1653,17 +1476,14 @@
       <c r="C63">
         <v>668928785514.92188</v>
       </c>
-      <c r="D63">
-        <v>5482612426.1889181</v>
+      <c r="D63" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E63" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F63" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>18600</v>
       </c>
@@ -1673,17 +1493,14 @@
       <c r="C64">
         <v>674436432701.04773</v>
       </c>
-      <c r="D64">
-        <v>4556326308.5222969</v>
+      <c r="D64" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E64" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F64" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>18900</v>
       </c>
@@ -1693,17 +1510,14 @@
       <c r="C65">
         <v>693462850253.1189</v>
       </c>
-      <c r="D65">
-        <v>1852572235.3332417</v>
+      <c r="D65" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E65" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F65" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>19200</v>
       </c>
@@ -1713,17 +1527,14 @@
       <c r="C66">
         <v>701223625833.56897</v>
       </c>
-      <c r="D66">
-        <v>4706534868.1439114</v>
+      <c r="D66" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E66" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F66" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>19500</v>
       </c>
@@ -1733,17 +1544,14 @@
       <c r="C67">
         <v>692461459855.64148</v>
       </c>
-      <c r="D67">
-        <v>5057021507.2610121</v>
+      <c r="D67" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E67" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F67" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>19800</v>
       </c>
@@ -1753,17 +1561,14 @@
       <c r="C68">
         <v>674436432701.04773</v>
       </c>
-      <c r="D68">
-        <v>5732960025.5582752</v>
+      <c r="D68" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E68" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F68" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>20100</v>
       </c>
@@ -1773,17 +1578,14 @@
       <c r="C69">
         <v>663671485928.16541</v>
       </c>
-      <c r="D69">
-        <v>7485393221.143774</v>
+      <c r="D69" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E69" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F69" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>20400</v>
       </c>
@@ -1793,17 +1595,14 @@
       <c r="C70">
         <v>648900977565.37341</v>
       </c>
-      <c r="D70">
-        <v>6859524222.7203817</v>
+      <c r="D70" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E70" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F70" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>20700</v>
       </c>
@@ -1813,17 +1612,14 @@
       <c r="C71">
         <v>647899587167.89587</v>
       </c>
-      <c r="D71">
-        <v>4331013469.0898752</v>
+      <c r="D71" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E71" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F71" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>21000</v>
       </c>
@@ -1833,17 +1629,14 @@
       <c r="C72">
         <v>676188865896.6333</v>
       </c>
-      <c r="D72">
-        <v>500695198.73871398</v>
+      <c r="D72" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E72" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F72" s="1">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>21300</v>
       </c>
@@ -1853,14 +1646,1898 @@
       <c r="C73">
         <v>654909319950.23792</v>
       </c>
-      <c r="D73">
-        <v>1276772756.7837205</v>
+      <c r="D73" s="1">
+        <v>100000000000</v>
       </c>
       <c r="E73" s="1">
         <v>1000000000</v>
       </c>
-      <c r="F73" s="1">
-        <v>10000000000</v>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>86400</v>
+      </c>
+      <c r="B74">
+        <v>346230729927.82074</v>
+      </c>
+      <c r="C74">
+        <v>678441994290.95752</v>
+      </c>
+      <c r="D74">
+        <v>100000000000</v>
+      </c>
+      <c r="E74">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>86700</v>
+      </c>
+      <c r="B75">
+        <v>354742548306.37885</v>
+      </c>
+      <c r="C75">
+        <v>692461459855.64148</v>
+      </c>
+      <c r="D75">
+        <v>100000000000</v>
+      </c>
+      <c r="E75">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>87000</v>
+      </c>
+      <c r="B76">
+        <v>359499152694.39661</v>
+      </c>
+      <c r="C76">
+        <v>710236139410.86584</v>
+      </c>
+      <c r="D76">
+        <v>100000000000</v>
+      </c>
+      <c r="E76">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>87300</v>
+      </c>
+      <c r="B77">
+        <v>364506104681.78381</v>
+      </c>
+      <c r="C77">
+        <v>680695122685.28174</v>
+      </c>
+      <c r="D77">
+        <v>100000000000</v>
+      </c>
+      <c r="E77">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>87600</v>
+      </c>
+      <c r="B78">
+        <v>365257147479.89185</v>
+      </c>
+      <c r="C78">
+        <v>654909319950.23792</v>
+      </c>
+      <c r="D78">
+        <v>100000000000</v>
+      </c>
+      <c r="E78">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>87900</v>
+      </c>
+      <c r="B79">
+        <v>366258537877.36932</v>
+      </c>
+      <c r="C79">
+        <v>674436432701.04773</v>
+      </c>
+      <c r="D79">
+        <v>100000000000</v>
+      </c>
+      <c r="E79">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>88200</v>
+      </c>
+      <c r="B80">
+        <v>354492200707.00952</v>
+      </c>
+      <c r="C80">
+        <v>706480925420.32544</v>
+      </c>
+      <c r="D80">
+        <v>100000000000</v>
+      </c>
+      <c r="E80">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>88500</v>
+      </c>
+      <c r="B81">
+        <v>342976211136.01904</v>
+      </c>
+      <c r="C81">
+        <v>728010818966.09009</v>
+      </c>
+      <c r="D81">
+        <v>100000000000</v>
+      </c>
+      <c r="E81">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>88800</v>
+      </c>
+      <c r="B82">
+        <v>345479687129.71265</v>
+      </c>
+      <c r="C82">
+        <v>735521246947.17078</v>
+      </c>
+      <c r="D82">
+        <v>100000000000</v>
+      </c>
+      <c r="E82">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>89100</v>
+      </c>
+      <c r="B83">
+        <v>348233510722.77557</v>
+      </c>
+      <c r="C83">
+        <v>732266728155.36926</v>
+      </c>
+      <c r="D83">
+        <v>100000000000</v>
+      </c>
+      <c r="E83">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>89400</v>
+      </c>
+      <c r="B84">
+        <v>364506104681.78381</v>
+      </c>
+      <c r="C84">
+        <v>715493438997.62219</v>
+      </c>
+      <c r="D84">
+        <v>100000000000</v>
+      </c>
+      <c r="E84">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>89700</v>
+      </c>
+      <c r="B85">
+        <v>380528351041.42261</v>
+      </c>
+      <c r="C85">
+        <v>672433651906.0929</v>
+      </c>
+      <c r="D85">
+        <v>100000000000</v>
+      </c>
+      <c r="E85">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>90000</v>
+      </c>
+      <c r="B86">
+        <v>374770356255.92743</v>
+      </c>
+      <c r="C86">
+        <v>651654801158.43628</v>
+      </c>
+      <c r="D86">
+        <v>100000000000</v>
+      </c>
+      <c r="E86">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>90300</v>
+      </c>
+      <c r="B87">
+        <v>368762013871.06287</v>
+      </c>
+      <c r="C87">
+        <v>662169400331.94922</v>
+      </c>
+      <c r="D87">
+        <v>100000000000</v>
+      </c>
+      <c r="E87">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>90600</v>
+      </c>
+      <c r="B88">
+        <v>373518618259.08063</v>
+      </c>
+      <c r="C88">
+        <v>662419747931.3186</v>
+      </c>
+      <c r="D88">
+        <v>100000000000</v>
+      </c>
+      <c r="E88">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>90900</v>
+      </c>
+      <c r="B89">
+        <v>378275222647.09839</v>
+      </c>
+      <c r="C89">
+        <v>673685389902.9397</v>
+      </c>
+      <c r="D89">
+        <v>100000000000</v>
+      </c>
+      <c r="E89">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>91200</v>
+      </c>
+      <c r="B90">
+        <v>389290517019.35016</v>
+      </c>
+      <c r="C90">
+        <v>678942689489.69617</v>
+      </c>
+      <c r="D90">
+        <v>100000000000</v>
+      </c>
+      <c r="E90">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>91500</v>
+      </c>
+      <c r="B91">
+        <v>400305811391.60187</v>
+      </c>
+      <c r="C91">
+        <v>659665924338.25574</v>
+      </c>
+      <c r="D91">
+        <v>100000000000</v>
+      </c>
+      <c r="E91">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91800</v>
+      </c>
+      <c r="B92">
+        <v>373268270659.7113</v>
+      </c>
+      <c r="C92">
+        <v>678191646691.58813</v>
+      </c>
+      <c r="D92">
+        <v>100000000000</v>
+      </c>
+      <c r="E92">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92100</v>
+      </c>
+      <c r="B93">
+        <v>346481077527.19006</v>
+      </c>
+      <c r="C93">
+        <v>689206941063.83984</v>
+      </c>
+      <c r="D93">
+        <v>100000000000</v>
+      </c>
+      <c r="E93">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>92400</v>
+      </c>
+      <c r="B94">
+        <v>362002628688.09021</v>
+      </c>
+      <c r="C94">
+        <v>657663143543.30078</v>
+      </c>
+      <c r="D94">
+        <v>100000000000</v>
+      </c>
+      <c r="E94">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>92700</v>
+      </c>
+      <c r="B95">
+        <v>377774527448.35968</v>
+      </c>
+      <c r="C95">
+        <v>654658972350.86853</v>
+      </c>
+      <c r="D95">
+        <v>100000000000</v>
+      </c>
+      <c r="E95">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>93000</v>
+      </c>
+      <c r="B96">
+        <v>369513056669.1709</v>
+      </c>
+      <c r="C96">
+        <v>675187475499.15576</v>
+      </c>
+      <c r="D96">
+        <v>100000000000</v>
+      </c>
+      <c r="E96">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>93300</v>
+      </c>
+      <c r="B97">
+        <v>361501933489.3515</v>
+      </c>
+      <c r="C97">
+        <v>680194427486.54297</v>
+      </c>
+      <c r="D97">
+        <v>100000000000</v>
+      </c>
+      <c r="E97">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>93600</v>
+      </c>
+      <c r="B98">
+        <v>355994286303.22565</v>
+      </c>
+      <c r="C98">
+        <v>682697903480.23657</v>
+      </c>
+      <c r="D98">
+        <v>100000000000</v>
+      </c>
+      <c r="E98">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>93900</v>
+      </c>
+      <c r="B99">
+        <v>350486639117.09979</v>
+      </c>
+      <c r="C99">
+        <v>702725711429.78503</v>
+      </c>
+      <c r="D99">
+        <v>100000000000</v>
+      </c>
+      <c r="E99">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>94200</v>
+      </c>
+      <c r="B100">
+        <v>372517227861.60321</v>
+      </c>
+      <c r="C100">
+        <v>695465631048.07373</v>
+      </c>
+      <c r="D100">
+        <v>100000000000</v>
+      </c>
+      <c r="E100">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>94500</v>
+      </c>
+      <c r="B101">
+        <v>394547816606.10663</v>
+      </c>
+      <c r="C101">
+        <v>679193037089.06555</v>
+      </c>
+      <c r="D101">
+        <v>100000000000</v>
+      </c>
+      <c r="E101">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>94800</v>
+      </c>
+      <c r="B102">
+        <v>386787041025.65656</v>
+      </c>
+      <c r="C102">
+        <v>692711807455.01086</v>
+      </c>
+      <c r="D102">
+        <v>100000000000</v>
+      </c>
+      <c r="E102">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>95100</v>
+      </c>
+      <c r="B103">
+        <v>379026265445.20648</v>
+      </c>
+      <c r="C103">
+        <v>702225016231.04639</v>
+      </c>
+      <c r="D103">
+        <v>100000000000</v>
+      </c>
+      <c r="E103">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>95400</v>
+      </c>
+      <c r="B104">
+        <v>384033217432.59363</v>
+      </c>
+      <c r="C104">
+        <v>698720149839.87537</v>
+      </c>
+      <c r="D104">
+        <v>100000000000</v>
+      </c>
+      <c r="E104">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>95700</v>
+      </c>
+      <c r="B105">
+        <v>389290517019.35016</v>
+      </c>
+      <c r="C105">
+        <v>702725711429.78503</v>
+      </c>
+      <c r="D105">
+        <v>100000000000</v>
+      </c>
+      <c r="E105">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>96000</v>
+      </c>
+      <c r="B106">
+        <v>387287736224.39526</v>
+      </c>
+      <c r="C106">
+        <v>714241701000.77551</v>
+      </c>
+      <c r="D106">
+        <v>100000000000</v>
+      </c>
+      <c r="E106">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>96300</v>
+      </c>
+      <c r="B107">
+        <v>385284955429.44043</v>
+      </c>
+      <c r="C107">
+        <v>706230577820.95605</v>
+      </c>
+      <c r="D107">
+        <v>100000000000</v>
+      </c>
+      <c r="E107">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>96600</v>
+      </c>
+      <c r="B108">
+        <v>376773137050.88232</v>
+      </c>
+      <c r="C108">
+        <v>704478144625.37061</v>
+      </c>
+      <c r="D108">
+        <v>100000000000</v>
+      </c>
+      <c r="E108">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>96900</v>
+      </c>
+      <c r="B109">
+        <v>368261318672.32416</v>
+      </c>
+      <c r="C109">
+        <v>714241701000.77551</v>
+      </c>
+      <c r="D109">
+        <v>100000000000</v>
+      </c>
+      <c r="E109">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>97200</v>
+      </c>
+      <c r="B110">
+        <v>385034607830.07111</v>
+      </c>
+      <c r="C110">
+        <v>698970497439.24475</v>
+      </c>
+      <c r="D110">
+        <v>100000000000</v>
+      </c>
+      <c r="E110">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>97500</v>
+      </c>
+      <c r="B111">
+        <v>401557549388.44861</v>
+      </c>
+      <c r="C111">
+        <v>688205550666.3623</v>
+      </c>
+      <c r="D111">
+        <v>100000000000</v>
+      </c>
+      <c r="E111">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>97800</v>
+      </c>
+      <c r="B112">
+        <v>394297469006.73724</v>
+      </c>
+      <c r="C112">
+        <v>701473973432.93823</v>
+      </c>
+      <c r="D112">
+        <v>100000000000</v>
+      </c>
+      <c r="E112">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>98100</v>
+      </c>
+      <c r="B113">
+        <v>387037388625.02594</v>
+      </c>
+      <c r="C113">
+        <v>696216673846.18176</v>
+      </c>
+      <c r="D113">
+        <v>100000000000</v>
+      </c>
+      <c r="E113">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>98400</v>
+      </c>
+      <c r="B114">
+        <v>364005409483.04504</v>
+      </c>
+      <c r="C114">
+        <v>706731273019.69482</v>
+      </c>
+      <c r="D114">
+        <v>100000000000</v>
+      </c>
+      <c r="E114">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>98700</v>
+      </c>
+      <c r="B115">
+        <v>340723082741.69489</v>
+      </c>
+      <c r="C115">
+        <v>732767423354.10791</v>
+      </c>
+      <c r="D115">
+        <v>100000000000</v>
+      </c>
+      <c r="E115">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>99000</v>
+      </c>
+      <c r="B116">
+        <v>345479687129.71265</v>
+      </c>
+      <c r="C116">
+        <v>731014990158.52246</v>
+      </c>
+      <c r="D116">
+        <v>100000000000</v>
+      </c>
+      <c r="E116">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>99300</v>
+      </c>
+      <c r="B117">
+        <v>350236291517.73047</v>
+      </c>
+      <c r="C117">
+        <v>693963545451.85754</v>
+      </c>
+      <c r="D117">
+        <v>100000000000</v>
+      </c>
+      <c r="E117">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>99600</v>
+      </c>
+      <c r="B118">
+        <v>347232120325.29816</v>
+      </c>
+      <c r="C118">
+        <v>664923223925.01208</v>
+      </c>
+      <c r="D118">
+        <v>100000000000</v>
+      </c>
+      <c r="E118">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>99900</v>
+      </c>
+      <c r="B119">
+        <v>343977601533.49652</v>
+      </c>
+      <c r="C119">
+        <v>682447555880.86719</v>
+      </c>
+      <c r="D119">
+        <v>100000000000</v>
+      </c>
+      <c r="E119">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>100200</v>
+      </c>
+      <c r="B120">
+        <v>338219606748.00128</v>
+      </c>
+      <c r="C120">
+        <v>702725711429.78503</v>
+      </c>
+      <c r="D120">
+        <v>100000000000</v>
+      </c>
+      <c r="E120">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>100500</v>
+      </c>
+      <c r="B121">
+        <v>332211264363.13672</v>
+      </c>
+      <c r="C121">
+        <v>695715978647.44312</v>
+      </c>
+      <c r="D121">
+        <v>100000000000</v>
+      </c>
+      <c r="E121">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>100800</v>
+      </c>
+      <c r="B122">
+        <v>347232120325.29816</v>
+      </c>
+      <c r="C122">
+        <v>667426699918.70581</v>
+      </c>
+      <c r="D122">
+        <v>100000000000</v>
+      </c>
+      <c r="E122">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>101100</v>
+      </c>
+      <c r="B123">
+        <v>362503323886.82892</v>
+      </c>
+      <c r="C123">
+        <v>663170790729.42664</v>
+      </c>
+      <c r="D123">
+        <v>100000000000</v>
+      </c>
+      <c r="E123">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>101400</v>
+      </c>
+      <c r="B124">
+        <v>357997067098.18054</v>
+      </c>
+      <c r="C124">
+        <v>678942689489.69617</v>
+      </c>
+      <c r="D124">
+        <v>100000000000</v>
+      </c>
+      <c r="E124">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>101700</v>
+      </c>
+      <c r="B125">
+        <v>353490810309.53204</v>
+      </c>
+      <c r="C125">
+        <v>702976059029.15442</v>
+      </c>
+      <c r="D125">
+        <v>100000000000</v>
+      </c>
+      <c r="E125">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>102000</v>
+      </c>
+      <c r="B126">
+        <v>350736986716.46912</v>
+      </c>
+      <c r="C126">
+        <v>725256995373.02722</v>
+      </c>
+      <c r="D126">
+        <v>100000000000</v>
+      </c>
+      <c r="E126">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>102300</v>
+      </c>
+      <c r="B127">
+        <v>347983163123.40625</v>
+      </c>
+      <c r="C127">
+        <v>713991353401.40613</v>
+      </c>
+      <c r="D127">
+        <v>100000000000</v>
+      </c>
+      <c r="E127">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>102600</v>
+      </c>
+      <c r="B128">
+        <v>350987334315.8385</v>
+      </c>
+      <c r="C128">
+        <v>696717369044.92053</v>
+      </c>
+      <c r="D128">
+        <v>100000000000</v>
+      </c>
+      <c r="E128">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>102900</v>
+      </c>
+      <c r="B129">
+        <v>354241853107.64014</v>
+      </c>
+      <c r="C129">
+        <v>678191646691.58813</v>
+      </c>
+      <c r="D129">
+        <v>100000000000</v>
+      </c>
+      <c r="E129">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>103200</v>
+      </c>
+      <c r="B130">
+        <v>349735596318.99176</v>
+      </c>
+      <c r="C130">
+        <v>667426699918.70581</v>
+      </c>
+      <c r="D130">
+        <v>100000000000</v>
+      </c>
+      <c r="E130">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>103500</v>
+      </c>
+      <c r="B131">
+        <v>345229339530.34326</v>
+      </c>
+      <c r="C131">
+        <v>653407234354.02185</v>
+      </c>
+      <c r="D131">
+        <v>100000000000</v>
+      </c>
+      <c r="E131">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>103800</v>
+      </c>
+      <c r="B132">
+        <v>341724473139.1723</v>
+      </c>
+      <c r="C132">
+        <v>638636725991.22974</v>
+      </c>
+      <c r="D132">
+        <v>100000000000</v>
+      </c>
+      <c r="E132">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>104100</v>
+      </c>
+      <c r="B133">
+        <v>338219606748.00128</v>
+      </c>
+      <c r="C133">
+        <v>673935737502.30908</v>
+      </c>
+      <c r="D133">
+        <v>100000000000</v>
+      </c>
+      <c r="E133">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>104400</v>
+      </c>
+      <c r="B134">
+        <v>350987334315.8385</v>
+      </c>
+      <c r="C134">
+        <v>692461459855.64148</v>
+      </c>
+      <c r="D134">
+        <v>100000000000</v>
+      </c>
+      <c r="E134">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>104700</v>
+      </c>
+      <c r="B135">
+        <v>364005409483.04504</v>
+      </c>
+      <c r="C135">
+        <v>668928785514.92188</v>
+      </c>
+      <c r="D135">
+        <v>100000000000</v>
+      </c>
+      <c r="E135">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>105000</v>
+      </c>
+      <c r="B136">
+        <v>347732815524.03687</v>
+      </c>
+      <c r="C136">
+        <v>674436432701.04773</v>
+      </c>
+      <c r="D136">
+        <v>100000000000</v>
+      </c>
+      <c r="E136">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>105300</v>
+      </c>
+      <c r="B137">
+        <v>331460221565.02869</v>
+      </c>
+      <c r="C137">
+        <v>693462850253.1189</v>
+      </c>
+      <c r="D137">
+        <v>100000000000</v>
+      </c>
+      <c r="E137">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>105600</v>
+      </c>
+      <c r="B138">
+        <v>326453269577.64148</v>
+      </c>
+      <c r="C138">
+        <v>701223625833.56897</v>
+      </c>
+      <c r="D138">
+        <v>100000000000</v>
+      </c>
+      <c r="E138">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>105900</v>
+      </c>
+      <c r="B139">
+        <v>321446317590.25439</v>
+      </c>
+      <c r="C139">
+        <v>692461459855.64148</v>
+      </c>
+      <c r="D139">
+        <v>100000000000</v>
+      </c>
+      <c r="E139">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>106200</v>
+      </c>
+      <c r="B140">
+        <v>325702226779.53345</v>
+      </c>
+      <c r="C140">
+        <v>674436432701.04773</v>
+      </c>
+      <c r="D140">
+        <v>100000000000</v>
+      </c>
+      <c r="E140">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>106500</v>
+      </c>
+      <c r="B141">
+        <v>329958135968.8125</v>
+      </c>
+      <c r="C141">
+        <v>663671485928.16541</v>
+      </c>
+      <c r="D141">
+        <v>100000000000</v>
+      </c>
+      <c r="E141">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>106800</v>
+      </c>
+      <c r="B142">
+        <v>338219606748.00128</v>
+      </c>
+      <c r="C142">
+        <v>648900977565.37341</v>
+      </c>
+      <c r="D142">
+        <v>100000000000</v>
+      </c>
+      <c r="E142">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>107100</v>
+      </c>
+      <c r="B143">
+        <v>346481077527.19006</v>
+      </c>
+      <c r="C143">
+        <v>647899587167.89587</v>
+      </c>
+      <c r="D143">
+        <v>100000000000</v>
+      </c>
+      <c r="E143">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>107400</v>
+      </c>
+      <c r="B144">
+        <v>325952574378.90277</v>
+      </c>
+      <c r="C144">
+        <v>676188865896.6333</v>
+      </c>
+      <c r="D144">
+        <v>100000000000</v>
+      </c>
+      <c r="E144">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>107700</v>
+      </c>
+      <c r="B145">
+        <v>305424071230.61554</v>
+      </c>
+      <c r="C145">
+        <v>654909319950.23792</v>
+      </c>
+      <c r="D145">
+        <v>100000000000</v>
+      </c>
+      <c r="E145">
+        <v>1000000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172C4B10-34B1-DA4C-872D-C5918B25BFA3}">
+  <dimension ref="A1:B72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <f>A1+86400</f>
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>300</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B65" si="0">A2+86400</f>
+        <v>86700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>600</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>900</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>87300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1200</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>87600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1500</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>87900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1800</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>88200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2100</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>88500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2400</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>88800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2700</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>89100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3000</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>89400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3300</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>89700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3600</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3900</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>90300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4200</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>90600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4500</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>90900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4800</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>91200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>5100</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>91500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>5400</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>91800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5700</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>92100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6000</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>92400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>6300</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>92700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6600</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>93000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6900</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>93300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>7200</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>93600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>7500</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>93900</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>7800</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>94200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>8100</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>94500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>8400</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>94800</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>8700</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>95100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>9000</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>95400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>9300</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>95700</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>9600</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>9900</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>96300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>10200</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>96600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>10500</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>96900</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>10800</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>97200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>11100</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>97500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>11400</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>97800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>11700</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>98100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>12000</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>98400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>12300</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>98700</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>12600</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>99000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>12900</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>99300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>13200</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>99600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>13500</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>99900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>13800</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>100200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>14100</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>100500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>14400</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>100800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>14700</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>101100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>15000</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>101400</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>15300</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>101700</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>15600</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>15900</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>102300</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>16200</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>102600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>16500</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>102900</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>16800</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>103200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>17100</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>103500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>17400</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>103800</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>17700</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>104100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>18000</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>104400</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>18300</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>104700</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>18600</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>18900</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>105300</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>19200</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>105600</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>19500</v>
+      </c>
+      <c r="B66">
+        <f t="shared" ref="B66:B72" si="1">A66+86400</f>
+        <v>105900</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>19800</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="1"/>
+        <v>106200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>20100</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>106500</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>20400</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>106800</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>20700</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>107100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>21000</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>107400</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>21300</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>107700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>